<commit_message>
Done reports, modifyed table
</commit_message>
<xml_diff>
--- a/report/data.xlsx
+++ b/report/data.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,14 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Inst\3 course\5 sem\par_prog\labs\5\par_prog-5\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{81105C95-C830-41BC-B3D0-87F953CFB48E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{974D7F26-FABC-4E21-A06F-3DAF32C78A0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -46,7 +57,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -859,6 +870,3130 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Avg</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> time</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="ru-RU" baseline="0"/>
+              <a:t> (µ</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>s)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Practical</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$F$2:$F$17</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>27941.46</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18067.21</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15862.559999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14760.419999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15727.239999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12038.919999999998</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12725.8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14246.39</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16012.060000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>15317.700000000003</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>16766.129999999997</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>14993.66</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>16423.129999999997</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14368.679999999998</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16238.679999999998</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>17238.109999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-FDE9-41FB-969D-BE6D2B7BD236}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Theoretical</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$G$2:$G$17</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>27941.46</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13970.73</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9313.82</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6985.3649999999998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5588.2919999999995</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4656.91</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3991.6371428571429</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3492.6824999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3104.6066666666666</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2794.1459999999997</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2540.1327272727272</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2328.4549999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2149.3430769230768</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1995.8185714285714</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1862.7639999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1746.3412499999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-FDE9-41FB-969D-BE6D2B7BD236}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="208269808"/>
+        <c:axId val="208268728"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="208269808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="208268728"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="208268728"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="28000"/>
+          <c:min val="1000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="208269808"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Avg speed</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> up</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Practical</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$H$2:$H$17</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5465287667548007</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.7614722970315009</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.8929989797038298</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.7766283213074898</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.3209274586092441</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.1956544971632432</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.961301073464927</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.7450259367002121</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.8241289488630796</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.6665420105892059</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.8635516611687872</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.7013480377979109</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.9446086905686537</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.7206731088980141</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.6209120373405208</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-74B6-4480-B2B6-2CCA4838361D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Theoretical</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$I$2:$I$17</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-74B6-4480-B2B6-2CCA4838361D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="603073296"/>
+        <c:axId val="603071136"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="603073296"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="603071136"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="603071136"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="16.5"/>
+          <c:min val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="603073296"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Avg efficiency</a:t>
+            </a:r>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Practical</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$J$2:$J$17</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.77326438337740033</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.58715743234383366</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.47324974492595745</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.35532566426149798</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.3868212431015407</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.31366492816617758</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.24516263418311587</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.19389177074446801</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.18241289488630796</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.15150381914447328</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.15529597176406559</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.13087292598445469</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.13890062075490384</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.11471154059320093</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.10130700233378255</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2D8A-4658-B9F1-52ED6C47C847}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Theoretical</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>data!$K$2:$K$17</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2D8A-4658-B9F1-52ED6C47C847}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="646175336"/>
+        <c:axId val="646176416"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="646175336"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="646176416"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="646176416"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1.1000000000000001"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="646175336"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>80962</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Диаграмма 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32D4B518-D8CE-0671-B938-761C9EBFC018}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Диаграмма 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{690CF2A8-ADCA-017D-EB43-C1EB2B10DE3B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>595312</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>404812</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Диаграмма 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2850999D-C508-878F-FB81-E7C36D40CC53}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
@@ -1155,11 +4290,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L160"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1279,7 +4414,7 @@
         <v>18067.21</v>
       </c>
       <c r="G3" s="14">
-        <f t="shared" ref="G3:G17" si="1">F$2/E3</f>
+        <f t="shared" ref="G3:G16" si="1">F$2/E3</f>
         <v>13970.73</v>
       </c>
       <c r="H3" s="17">
@@ -1361,7 +4496,7 @@
         <v>4</v>
       </c>
       <c r="F5" s="11">
-        <f t="shared" ref="F3:F17" si="5">SUMIF(D:D, E5,C:C)/$L$1</f>
+        <f t="shared" ref="F5:F17" si="5">SUMIF(D:D, E5,C:C)/$L$1</f>
         <v>14760.419999999998</v>
       </c>
       <c r="G5" s="14">
@@ -4033,5 +7168,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>